<commit_message>
Weiter an Kopfrechnen gearbeitet
</commit_message>
<xml_diff>
--- a/Zeiterfassung.xlsx
+++ b/Zeiterfassung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thisi\OneDrive\Desktop\Programme\ema\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60BFAE03-D608-4711-9C4B-3D9A994E6977}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B4F9C6F-C8A2-4439-A967-C44C92316245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="1575" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeiterfassung" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1038" uniqueCount="37">
   <si>
     <t>Summe (h)</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>6. Vorlesung</t>
+  </si>
+  <si>
+    <t>5, 21</t>
+  </si>
+  <si>
+    <t>An Kopfrechnen gearbeitet</t>
   </si>
 </sst>
 </file>
@@ -3447,7 +3453,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3466,7 +3472,7 @@
       </c>
       <c r="C3" s="2">
         <f>SUM(C6:C300)</f>
-        <v>1.1111111111111107</v>
+        <v>1.2152777777777775</v>
       </c>
       <c r="D3" s="3"/>
     </row>
@@ -3689,7 +3695,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" t="s">
         <v>7</v>
@@ -3704,16 +3710,27 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="4"/>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="4">
+        <v>45250</v>
+      </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>15</v>
+      </c>
+      <c r="C18" s="5">
+        <v>0.10416666666666667</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" t="s">
         <v>24</v>
@@ -3722,7 +3739,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" t="s">
         <v>24</v>
@@ -3731,7 +3748,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" t="s">
         <v>24</v>
@@ -3740,7 +3757,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" t="s">
         <v>24</v>
@@ -3749,7 +3766,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" t="s">
         <v>24</v>
@@ -3758,7 +3775,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" t="s">
         <v>24</v>
@@ -3767,7 +3784,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" t="s">
         <v>24</v>
@@ -3776,7 +3793,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" t="s">
         <v>24</v>
@@ -3785,7 +3802,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" t="s">
         <v>24</v>
@@ -3794,7 +3811,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" t="s">
         <v>24</v>
@@ -3803,7 +3820,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" t="s">
         <v>24</v>
@@ -3812,7 +3829,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" t="s">
         <v>24</v>
@@ -3821,7 +3838,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" t="s">
         <v>24</v>
@@ -3830,7 +3847,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" t="s">
         <v>24</v>

</xml_diff>